<commit_message>
Cooreção cadastro Pessoa Física, select.js
</commit_message>
<xml_diff>
--- a/Projeto/DB Tableas.xlsx
+++ b/Projeto/DB Tableas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/delfos/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70242A6F-7597-114F-B314-B9496774FA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357B01DC-6133-1A49-9188-5C4196FB8959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="500" windowWidth="57600" windowHeight="35500" activeTab="5" xr2:uid="{65F3778F-F7A3-5945-852B-B3CE144BC84D}"/>
   </bookViews>
@@ -20430,7 +20430,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H78" sqref="H78"/>
+      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Antes mudar nome banco delfos para conectaidealcom_db
</commit_message>
<xml_diff>
--- a/Projeto/DB Tableas.xlsx
+++ b/Projeto/DB Tableas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/delfos/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A65077B-087B-6C49-B14B-3E8865D4B03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA983D20-F746-9E4B-AE94-66F3CEAE16C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="57600" windowHeight="35500" activeTab="4" xr2:uid="{65F3778F-F7A3-5945-852B-B3CE144BC84D}"/>
+    <workbookView xWindow="28880" yWindow="-35500" windowWidth="32000" windowHeight="35500" activeTab="4" xr2:uid="{65F3778F-F7A3-5945-852B-B3CE144BC84D}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="722">
   <si>
     <t>bsc_banco</t>
   </si>
@@ -2181,19 +2181,31 @@
     <t>tipo_arquivo, documento</t>
   </si>
   <si>
-    <t xml:space="preserve">  `internet_banda_larga_velocidade` varchar(50) DEFAULT NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  `alimentacao_pnae_fnde_oferece` tinyint(1) DEFAULT '0',</t>
-  </si>
-  <si>
     <t>$rsRegistrosUEEquipam</t>
   </si>
   <si>
-    <t>uee_</t>
-  </si>
-  <si>
-    <t>uee.</t>
+    <t xml:space="preserve">  `id` int(11) NOT NULL AUTO_INCREMENT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `status` tinyint(1) NOT NULL DEFAULT '0',</t>
+  </si>
+  <si>
+    <t>ue_</t>
+  </si>
+  <si>
+    <t>ue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `dt_cadastro` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `descricao` text,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `ue_ue_id` int(11) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `bsc_uo_publica_id` int(11) NOT NULL,</t>
   </si>
 </sst>
 </file>
@@ -2547,8 +2559,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2556,17 +2571,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14096,8 +14108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B488E7A0-5FC7-8C46-9378-12741E521CD7}">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14120,102 +14132,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="O2" t="str">
         <f>LEFT(L5,(41-LEN(G5)))</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                       </v>
       </c>
     </row>
     <row r="3" spans="1:19" s="39" customFormat="1" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>567</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>568</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="52" t="s">
         <v>310</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="52" t="s">
         <v>315</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="52" t="s">
         <v>316</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="52" t="s">
         <v>311</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="52" t="s">
         <v>312</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="52" t="s">
         <v>313</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="52" t="s">
         <v>317</v>
       </c>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="50" t="s">
         <v>570</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="50" t="s">
         <v>569</v>
       </c>
       <c r="N3" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="O3" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="P3" s="51" t="s">
+      <c r="P3" s="52" t="s">
         <v>319</v>
       </c>
-      <c r="Q3" s="51" t="s">
+      <c r="Q3" s="52" t="s">
         <v>321</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="52" t="s">
         <v>320</v>
       </c>
-      <c r="S3" s="55" t="s">
+      <c r="S3" s="54" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="39" customFormat="1" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
       <c r="N4" s="40" t="s">
-        <v>715</v>
-      </c>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="56"/>
+        <v>713</v>
+      </c>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="55"/>
     </row>
     <row r="5" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
@@ -14228,60 +14240,60 @@
         <v>717</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="13" t="str">
         <f t="shared" ref="G5:G32" si="0">IFERROR(MID(D5,(FIND("`",D5)+1),(FIND("` ",D5)-(FIND("`",D5)+1))),"")</f>
-        <v>internet_banda_larga_velocidade</v>
+        <v>id</v>
       </c>
       <c r="H5" s="13" t="str">
         <f>IFERROR(MID(D5,(FIND("` ",D5)+2),(IFERROR(FIND("NOT",D5),FIND("DEFAULT",D5))-(FIND("` ",D5)+3))),"")</f>
-        <v>varchar(50)</v>
+        <v>int(11)</v>
       </c>
       <c r="I5" s="13" t="str">
         <f t="shared" ref="I5:I32" si="1">IFERROR(MID(D5,(FIND("(",D5)+1),(FIND(")",D5)-(FIND("(",D5)+1))),"")</f>
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="J5" s="13" t="str">
         <f>IF((IFERROR(FIND("NOT NULL",D5),0))&gt;0,"true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="K5" s="13" t="str">
         <f>CONCATENATE(B5,G5,", ")</f>
-        <v xml:space="preserve">uee_internet_banda_larga_velocidade, </v>
+        <v xml:space="preserve">ue_id, </v>
       </c>
       <c r="L5" s="13" t="s">
         <v>571</v>
       </c>
       <c r="M5" s="13" t="str">
         <f>CONCATENATE(C5,G5,",")</f>
-        <v>uee.internet_banda_larga_velocidade,</v>
+        <v>ue.id,</v>
       </c>
       <c r="N5" s="13" t="str">
         <f>CONCATENATE(N$4,"['",G5,"'] = '';")</f>
-        <v>$rsRegistrosUEEquipam['internet_banda_larga_velocidade'] = '';</v>
+        <v>$rsRegistrosUEEquipam['id'] = '';</v>
       </c>
       <c r="O5" s="13" t="str">
         <f>CONCATENATE("'name' =&gt; '",B5,G5,"',    ","'id' =&gt; '",B5,G5,"',    ","'maxlength' =&gt; ",I5,",    ","'value' =&gt; ",N$4,"['",G5,"'],    ","'required' =&gt; ",J5)</f>
-        <v>'name' =&gt; 'uee_internet_banda_larga_velocidade',    'id' =&gt; 'uee_internet_banda_larga_velocidade',    'maxlength' =&gt; 50,    'value' =&gt; $rsRegistrosUEEquipam['internet_banda_larga_velocidade'],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_id',    'id' =&gt; 'ue_id',    'maxlength' =&gt; 11,    'value' =&gt; $rsRegistrosUEEquipam['id'],    'required' =&gt; true</v>
       </c>
       <c r="P5" s="13" t="str">
         <f>CONCATENATE("$",G5,LEFT(L5,(41-LEN(G5))),"= ",IF(OR(IFERROR(FIND("dt_",G5),0)&gt;0,IFERROR(FIND("_id",G5),0)&gt;0,G5="status"),"","ucwords(strtolower(trim("),"strip_tags(@$_POST['",B5,G5,"']?: ",IF(G5="status","0)","'')"),IF(OR(IFERROR(FIND("dt_",G5),0)&gt;0,IFERROR(FIND("_id",G5),0)&gt;0,G5="status"),";",")));"))</f>
-        <v>$internet_banda_larga_velocidade          = ucwords(strtolower(trim(strip_tags(@$_POST['uee_internet_banda_larga_velocidade']?: ''))));</v>
+        <v>$id                                       = ucwords(strtolower(trim(strip_tags(@$_POST['ue_id']?: ''))));</v>
       </c>
       <c r="Q5" s="13" t="str">
         <f>CONCATENATE(G5," = ?,")</f>
-        <v>internet_banda_larga_velocidade = ?,</v>
+        <v>id = ?,</v>
       </c>
       <c r="R5" s="13" t="str">
         <f t="shared" ref="R5:R36" si="2">CONCATENATE(G5,",")</f>
-        <v>internet_banda_larga_velocidade,</v>
+        <v>id,</v>
       </c>
       <c r="S5" s="14" t="str">
         <f t="shared" ref="S5:S25" si="3">CONCATENATE("$stmt-&gt;bindValue(",A5,", $",G5,IF(OR(IFERROR(FIND("dt_",G5),0)&gt;0,IFERROR(FIND("_id",G5),0)&gt;0,IFERROR(FIND("_ano",G5),0)&gt;0),"?: NULL);",");"))</f>
-        <v>$stmt-&gt;bindValue(1, $internet_banda_larga_velocidade);</v>
+        <v>$stmt-&gt;bindValue(1, $id);</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -14295,13 +14307,13 @@
         <v>717</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>alimentacao_pnae_fnde_oferece</v>
+        <v>status</v>
       </c>
       <c r="H6" s="9" t="str">
         <f t="shared" ref="H6:H32" si="4">IFERROR(MID(D6,(FIND("` ",D6)+2),(IFERROR(FIND("NOT",D6),FIND("DEFAULT",D6))-(FIND("` ",D6)+3))),"")</f>
@@ -14313,60 +14325,66 @@
       </c>
       <c r="J6" s="9" t="str">
         <f>IF((IFERROR(FIND("NOT NULL",D6),0))&gt;0,"true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="K6" s="9" t="str">
         <f t="shared" ref="K6:K69" si="5">CONCATENATE(B6,G6,", ")</f>
-        <v xml:space="preserve">uee_alimentacao_pnae_fnde_oferece, </v>
+        <v xml:space="preserve">ue_status, </v>
       </c>
       <c r="L6" s="9" t="s">
         <v>571</v>
       </c>
       <c r="M6" s="9" t="str">
         <f t="shared" ref="M6:M69" si="6">CONCATENATE(C6,G6,",")</f>
-        <v>uee.alimentacao_pnae_fnde_oferece,</v>
+        <v>ue.status,</v>
       </c>
       <c r="N6" s="9" t="str">
         <f t="shared" ref="N6:N69" si="7">CONCATENATE(N$4,"['",G6,"'] = '';")</f>
-        <v>$rsRegistrosUEEquipam['alimentacao_pnae_fnde_oferece'] = '';</v>
+        <v>$rsRegistrosUEEquipam['status'] = '';</v>
       </c>
       <c r="O6" s="9" t="str">
         <f t="shared" ref="O6:O69" si="8">CONCATENATE("'name' =&gt; '",B6,G6,"',    ","'id' =&gt; '",B6,G6,"',    ","'maxlength' =&gt; ",I6,",    ","'value' =&gt; ",N$4,"['",G6,"'],    ","'required' =&gt; ",J6)</f>
-        <v>'name' =&gt; 'uee_alimentacao_pnae_fnde_oferece',    'id' =&gt; 'uee_alimentacao_pnae_fnde_oferece',    'maxlength' =&gt; 1,    'value' =&gt; $rsRegistrosUEEquipam['alimentacao_pnae_fnde_oferece'],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_status',    'id' =&gt; 'ue_status',    'maxlength' =&gt; 1,    'value' =&gt; $rsRegistrosUEEquipam['status'],    'required' =&gt; true</v>
       </c>
       <c r="P6" s="13" t="str">
         <f t="shared" ref="P6:P69" si="9">CONCATENATE("$",G6,LEFT(L6,(41-LEN(G6))),"= ",IF(OR(IFERROR(FIND("dt_",G6),0)&gt;0,IFERROR(FIND("_id",G6),0)&gt;0,G6="status"),"","ucwords(strtolower(trim("),"strip_tags(@$_POST['",B6,G6,"']?: ",IF(G6="status","0)","'')"),IF(OR(IFERROR(FIND("dt_",G6),0)&gt;0,IFERROR(FIND("_id",G6),0)&gt;0,G6="status"),";",")));"))</f>
-        <v>$alimentacao_pnae_fnde_oferece            = ucwords(strtolower(trim(strip_tags(@$_POST['uee_alimentacao_pnae_fnde_oferece']?: ''))));</v>
+        <v>$status                                   = strip_tags(@$_POST['ue_status']?: 0);</v>
       </c>
       <c r="Q6" s="9" t="str">
         <f t="shared" ref="Q6:Q69" si="10">CONCATENATE(G6," = ?,")</f>
-        <v>alimentacao_pnae_fnde_oferece = ?,</v>
+        <v>status = ?,</v>
       </c>
       <c r="R6" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>alimentacao_pnae_fnde_oferece,</v>
+        <v>status,</v>
       </c>
       <c r="S6" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>$stmt-&gt;bindValue(2, $alimentacao_pnae_fnde_oferece);</v>
+        <v>$stmt-&gt;bindValue(2, $status);</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>718</v>
+      </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>dt_cadastro</v>
       </c>
       <c r="H7" s="9" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>timestamp</v>
       </c>
       <c r="I7" s="9" t="str">
         <f t="shared" si="1"/>
@@ -14374,56 +14392,62 @@
       </c>
       <c r="J7" s="9" t="str">
         <f t="shared" ref="J7:J70" si="11">IF((IFERROR(FIND("NOT NULL",D7),0))&gt;0,"true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="K7" s="9" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">, </v>
+        <v xml:space="preserve">ue_dt_cadastro, </v>
       </c>
       <c r="L7" s="9" t="s">
         <v>571</v>
       </c>
       <c r="M7" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>,</v>
+        <v>ue.dt_cadastro,</v>
       </c>
       <c r="N7" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>$rsRegistrosUEEquipam[''] = '';</v>
+        <v>$rsRegistrosUEEquipam['dt_cadastro'] = '';</v>
       </c>
       <c r="O7" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>'name' =&gt; '',    'id' =&gt; '',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam[''],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_dt_cadastro',    'id' =&gt; 'ue_dt_cadastro',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam['dt_cadastro'],    'required' =&gt; true</v>
       </c>
       <c r="P7" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>$                                         = ucwords(strtolower(trim(strip_tags(@$_POST['']?: ''))));</v>
+        <v>$dt_cadastro                              = strip_tags(@$_POST['ue_dt_cadastro']?: '');</v>
       </c>
       <c r="Q7" s="9" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve"> = ?,</v>
+        <v>dt_cadastro = ?,</v>
       </c>
       <c r="R7" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>,</v>
+        <v>dt_cadastro,</v>
       </c>
       <c r="S7" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>$stmt-&gt;bindValue(3, $);</v>
+        <v>$stmt-&gt;bindValue(3, $dt_cadastro?: NULL);</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>719</v>
+      </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>descricao</v>
       </c>
       <c r="H8" s="9" t="str">
         <f t="shared" si="4"/>
@@ -14439,160 +14463,172 @@
       </c>
       <c r="K8" s="9" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">, </v>
+        <v xml:space="preserve">ue_descricao, </v>
       </c>
       <c r="L8" s="9" t="s">
         <v>571</v>
       </c>
       <c r="M8" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>,</v>
+        <v>ue.descricao,</v>
       </c>
       <c r="N8" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>$rsRegistrosUEEquipam[''] = '';</v>
+        <v>$rsRegistrosUEEquipam['descricao'] = '';</v>
       </c>
       <c r="O8" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>'name' =&gt; '',    'id' =&gt; '',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam[''],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_descricao',    'id' =&gt; 'ue_descricao',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam['descricao'],    'required' =&gt; false</v>
       </c>
       <c r="P8" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>$                                         = ucwords(strtolower(trim(strip_tags(@$_POST['']?: ''))));</v>
+        <v>$descricao                                = ucwords(strtolower(trim(strip_tags(@$_POST['ue_descricao']?: ''))));</v>
       </c>
       <c r="Q8" s="9" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve"> = ?,</v>
+        <v>descricao = ?,</v>
       </c>
       <c r="R8" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>,</v>
+        <v>descricao,</v>
       </c>
       <c r="S8" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>$stmt-&gt;bindValue(4, $);</v>
+        <v>$stmt-&gt;bindValue(4, $descricao);</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>720</v>
+      </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>ue_ue_id</v>
       </c>
       <c r="H9" s="9" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>int(11)</v>
       </c>
       <c r="I9" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="J9" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="K9" s="9" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">, </v>
+        <v xml:space="preserve">ue_ue_ue_id, </v>
       </c>
       <c r="L9" s="9" t="s">
         <v>571</v>
       </c>
       <c r="M9" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>,</v>
+        <v>ue.ue_ue_id,</v>
       </c>
       <c r="N9" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>$rsRegistrosUEEquipam[''] = '';</v>
+        <v>$rsRegistrosUEEquipam['ue_ue_id'] = '';</v>
       </c>
       <c r="O9" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>'name' =&gt; '',    'id' =&gt; '',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam[''],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_ue_ue_id',    'id' =&gt; 'ue_ue_ue_id',    'maxlength' =&gt; 11,    'value' =&gt; $rsRegistrosUEEquipam['ue_ue_id'],    'required' =&gt; true</v>
       </c>
       <c r="P9" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>$                                         = ucwords(strtolower(trim(strip_tags(@$_POST['']?: ''))));</v>
+        <v>$ue_ue_id                                 = strip_tags(@$_POST['ue_ue_ue_id']?: '');</v>
       </c>
       <c r="Q9" s="9" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve"> = ?,</v>
+        <v>ue_ue_id = ?,</v>
       </c>
       <c r="R9" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>,</v>
+        <v>ue_ue_id,</v>
       </c>
       <c r="S9" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>$stmt-&gt;bindValue(5, $);</v>
+        <v>$stmt-&gt;bindValue(5, $ue_ue_id?: NULL);</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>6</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>721</v>
+      </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>bsc_uo_publica_id</v>
       </c>
       <c r="H10" s="9" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>int(11)</v>
       </c>
       <c r="I10" s="9" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="J10" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="K10" s="9" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">, </v>
+        <v xml:space="preserve">ue_bsc_uo_publica_id, </v>
       </c>
       <c r="L10" s="9" t="s">
         <v>571</v>
       </c>
       <c r="M10" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>,</v>
+        <v>ue.bsc_uo_publica_id,</v>
       </c>
       <c r="N10" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>$rsRegistrosUEEquipam[''] = '';</v>
+        <v>$rsRegistrosUEEquipam['bsc_uo_publica_id'] = '';</v>
       </c>
       <c r="O10" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>'name' =&gt; '',    'id' =&gt; '',    'maxlength' =&gt; ,    'value' =&gt; $rsRegistrosUEEquipam[''],    'required' =&gt; false</v>
+        <v>'name' =&gt; 'ue_bsc_uo_publica_id',    'id' =&gt; 'ue_bsc_uo_publica_id',    'maxlength' =&gt; 11,    'value' =&gt; $rsRegistrosUEEquipam['bsc_uo_publica_id'],    'required' =&gt; true</v>
       </c>
       <c r="P10" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>$                                         = ucwords(strtolower(trim(strip_tags(@$_POST['']?: ''))));</v>
+        <v>$bsc_uo_publica_id                        = strip_tags(@$_POST['ue_bsc_uo_publica_id']?: '');</v>
       </c>
       <c r="Q10" s="9" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve"> = ?,</v>
+        <v>bsc_uo_publica_id = ?,</v>
       </c>
       <c r="R10" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>,</v>
+        <v>bsc_uo_publica_id,</v>
       </c>
       <c r="S10" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>$stmt-&gt;bindValue(6, $);</v>
+        <v>$stmt-&gt;bindValue(6, $bsc_uo_publica_id?: NULL);</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -20332,6 +20368,14 @@
     <row r="105" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
@@ -20343,14 +20387,6 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>